<commit_message>
Delete Employee Info function
</commit_message>
<xml_diff>
--- a/employee_data.xlsx
+++ b/employee_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -479,25 +479,6 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>3</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>CSL</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>15</v>
-      </c>
-      <c r="D3" t="n">
-        <v>10</v>
-      </c>
-      <c r="E3" t="n">
-        <v>17</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Done Update Employee's Info Function
</commit_message>
<xml_diff>
--- a/employee_data.xlsx
+++ b/employee_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -470,13 +470,51 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="D2" t="n">
         <v>8</v>
       </c>
       <c r="E2" t="n">
         <v>35</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Tee</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>5</v>
+      </c>
+      <c r="D3" t="n">
+        <v>7</v>
+      </c>
+      <c r="E3" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>CSL</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>9</v>
+      </c>
+      <c r="D4" t="n">
+        <v>8</v>
+      </c>
+      <c r="E4" t="n">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Done Working Hours, Basic Structure of Generate Payslip function
</commit_message>
<xml_diff>
--- a/employee_data.xlsx
+++ b/employee_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -517,6 +517,27 @@
         <v>10</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>69</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Thim</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>2</v>
+      </c>
+      <c r="D5" t="n">
+        <v>24</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Delete astype(str) change to set int input for id
</commit_message>
<xml_diff>
--- a/employee_data.xlsx
+++ b/employee_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,7 +473,7 @@
         <v>80</v>
       </c>
       <c r="D2" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E2" t="n">
         <v>35</v>
@@ -515,27 +515,6 @@
       </c>
       <c r="E4" t="n">
         <v>10</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>69</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Thim</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>2</v>
-      </c>
-      <c r="D5" t="n">
-        <v>24</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add new database:payslip_data and Create a function to write generate payslip history into it
</commit_message>
<xml_diff>
--- a/employee_data.xlsx
+++ b/employee_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -517,6 +517,46 @@
         <v>10</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>RyanKho</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>5</v>
+      </c>
+      <c r="D5" t="n">
+        <v>5</v>
+      </c>
+      <c r="E5" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Thim</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>6</v>
+      </c>
+      <c r="D6" t="n">
+        <v>6</v>
+      </c>
+      <c r="E6" t="n">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix bug for ValueError in Add Employee function
</commit_message>
<xml_diff>
--- a/employee_data.xlsx
+++ b/employee_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -537,10 +537,8 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
+      <c r="A6" t="n">
+        <v>5</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -555,6 +553,27 @@
       </c>
       <c r="E6" t="n">
         <v>6</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Xi</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>10</v>
+      </c>
+      <c r="D7" t="n">
+        <v>10</v>
+      </c>
+      <c r="E7" t="n">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>